<commit_message>
some modification to the previous work
</commit_message>
<xml_diff>
--- a/Previous Work/genmix_new.xlsx
+++ b/Previous Work/genmix_new.xlsx
@@ -356,7 +356,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:J1022"/>
+  <dimension ref="A2:J1023"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H1007" sqref="H1007"/>
@@ -29829,6 +29829,31 @@
         <v>23</v>
       </c>
     </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>[(1, 228), (2, 36), (3, 259), (4, 98), (5, 403)]</t>
+        </is>
+      </c>
+      <c r="B1023" t="n">
+        <v>5</v>
+      </c>
+      <c r="C1023" t="n">
+        <v>32</v>
+      </c>
+      <c r="D1023" t="n">
+        <v>25</v>
+      </c>
+      <c r="E1023" t="n">
+        <v>22</v>
+      </c>
+      <c r="F1023" t="n">
+        <v>16</v>
+      </c>
+      <c r="G1023" t="n">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>